<commit_message>
weather, fish cost by time to game data
</commit_message>
<xml_diff>
--- a/게임 데이터 테이블 구성.xlsx
+++ b/게임 데이터 테이블 구성.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nayoonv\game-uruk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E501F779-9CB8-41C6-8C19-C023BAD114E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A38E31-7780-4A9C-AA1F-54124247C55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39460" yWindow="1060" windowWidth="28800" windowHeight="15500" xr2:uid="{5DE46ADA-ACE9-4313-BE07-D63152852563}"/>
+    <workbookView xWindow="15280" yWindow="4620" windowWidth="28800" windowHeight="15500" xr2:uid="{5DE46ADA-ACE9-4313-BE07-D63152852563}"/>
   </bookViews>
   <sheets>
     <sheet name="game" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="81">
   <si>
     <t>account_user</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -176,14 +176,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sold_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>got_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>획득 날짜</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -212,18 +204,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>판 날짜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cost</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>판매 가격</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>물고기를 사고 판 기록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -249,6 +233,130 @@
   </si>
   <si>
     <t>게임 플레이를 위한 사용자 정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inventory_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inventory_type_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inventory_type_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인벤토리 타입 이름(물고기인지 아이템인지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인벤토리 타입 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인벤토리 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 id (채비일 경우 item_id, 물고기일 경우 fish_id)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>누적 골드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>week</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주 (week(오늘 날짜) 함수를 사용해서 구하려고 합니다.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_weather</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저별 날씨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_fish_cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_fish_cost_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_weather_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind_direction_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wind_speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저 날씨 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풍향 id (1~8까지 랜덤 함수로부터 나온 값 저장)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풍속 (0~20까지 랜덤함수로부터 나온 값 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>온도 (0~30까지 랜덤 함수로부터 나온 값 저장)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저별 물고기 시세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저별 물고기 시세 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맵 id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가격 (희귀도, 어려운 맵, 크기에 따라 결정됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시간 (거래가 이루어지던 시간)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -322,7 +430,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -333,6 +441,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -649,17 +769,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41C1106-E51B-4FF6-A0D9-BA9386E07A59}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="2" width="31.58203125" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="3" max="3" width="48.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -667,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -730,7 +850,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -804,7 +924,7 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -819,14 +939,14 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="2">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>23</v>
+      <c r="A18" s="7">
+        <v>1</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -834,240 +954,446 @@
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>3</v>
+      <c r="B22" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="2">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>34</v>
+      <c r="A23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="2">
         <v>4</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>3</v>
+      <c r="B29" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" s="2">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>34</v>
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="2">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="2">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="7">
+        <v>1</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="7">
+        <v>2</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="2">
-        <v>1</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" s="2">
-        <v>2</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A38" s="2">
-        <v>3</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>3</v>
+      <c r="B41" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" s="2">
-        <v>1</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>34</v>
+      <c r="A42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
+        <v>3</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" s="2">
+        <v>1</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" s="2">
+        <v>2</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" s="2">
+        <v>3</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58">
         <v>4</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>46</v>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>